<commit_message>
Création du projet C# et fichier gitignore
</commit_message>
<xml_diff>
--- a/Matrice Implication PROGAV.xlsx
+++ b/Matrice Implication PROGAV.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8811928-F19F-4A1E-BEF3-44DD370959E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756BCE19-47AF-C44E-8AB1-238C567DCE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="6828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -15,19 +15,27 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>n°</t>
   </si>
   <si>
-    <t>date:</t>
-  </si>
-  <si>
     <t>REMARQUES:</t>
   </si>
   <si>
@@ -41,9 +49,6 @@
   </si>
   <si>
     <t>Nom du/des Codeurs</t>
-  </si>
-  <si>
-    <t>MEMBRES DE L'EQUIPE:</t>
   </si>
   <si>
     <t>Nom 
@@ -51,6 +56,15 @@
   </si>
   <si>
     <t>MATRICE D'IMPLICATION : PROJET PROGAV</t>
+  </si>
+  <si>
+    <t>MEMBRES DE L'EQUIPE : AMMAR-BOUDJELAL Lina</t>
+  </si>
+  <si>
+    <t>date : 23/05/2025</t>
+  </si>
+  <si>
+    <t>ENSemenC</t>
   </si>
 </sst>
 </file>
@@ -382,6 +396,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,21 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,232 +726,234 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="11.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="11.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="41.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+    <row r="1" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="2:5" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26" t="s">
+    </row>
+    <row r="5" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <f>1+B7</f>
         <v>2</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="29"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
         <f t="shared" ref="B9:B21" si="0">1+B8</f>
         <v>3</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="29"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="29"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="29"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="29"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="29"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="29"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="29"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="29"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="29"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="29"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="29"/>
-    </row>
-    <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="18"/>
+    </row>
+    <row r="21" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="30"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="10"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="10"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="10"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="10"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="10"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>

</xml_diff>

<commit_message>
Ajout du rapport technique et de la matrice d'implication
</commit_message>
<xml_diff>
--- a/Matrice Implication PROGAV.xlsx
+++ b/Matrice Implication PROGAV.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756BCE19-47AF-C44E-8AB1-238C567DCE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD800365-6F2F-D04D-A16B-F59593466A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16160" yWindow="760" windowWidth="14080" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,21 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>n°</t>
   </si>
   <si>
-    <t>REMARQUES:</t>
-  </si>
-  <si>
     <t>Pourcentage de participation si tâche partagée</t>
   </si>
   <si>
     <t>Tâche/Fonctionnalité/Fonction</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>Nom du/des Codeurs</t>
@@ -65,13 +59,67 @@
   </si>
   <si>
     <t>ENSemenC</t>
+  </si>
+  <si>
+    <r>
+      <t>REMARQUES :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Projet réalisé en autonomie.</t>
+    </r>
+  </si>
+  <si>
+    <t>Analyse du sujet</t>
+  </si>
+  <si>
+    <t>Conception des classes principales et description de l'univers du jeu (UML, modélisation)</t>
+  </si>
+  <si>
+    <t>Création des classes de monde</t>
+  </si>
+  <si>
+    <t>Création des classes de plantes</t>
+  </si>
+  <si>
+    <t>Création de la classe simulation et boucle de jeu</t>
+  </si>
+  <si>
+    <t>Création des classes météo et terrain</t>
+  </si>
+  <si>
+    <t>Systèmes de maladies et soins</t>
+  </si>
+  <si>
+    <t>Gestion des urgences et nuisibles</t>
+  </si>
+  <si>
+    <t>Actions joueurs (semis, arrosage, etc.)</t>
+  </si>
+  <si>
+    <t>Interface console et affichage stylisé</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport</t>
+  </si>
+  <si>
+    <t>README et documentation</t>
+  </si>
+  <si>
+    <t>AMMAR-BOUDJELAL Lina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +128,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -89,15 +136,7 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -112,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -335,114 +374,95 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,246 +744,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E28"/>
+  <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1"/>
-    <col min="2" max="2" width="11.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.83203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="8"/>
+    <col min="2" max="2" width="7" style="8" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="2:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="2:5" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+    </row>
+    <row r="5" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="18">
+        <v>1</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="4">
+      <c r="D7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="18">
         <f>1+B7</f>
         <v>2</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
-        <f t="shared" ref="B9:B21" si="0">1+B8</f>
+      <c r="C8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="18">
+        <f t="shared" ref="B9:B18" si="0">1+B8</f>
         <v>3</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="4">
+      <c r="C9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="4">
+      <c r="C10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
+      <c r="C11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="4">
+      <c r="C12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="4">
+      <c r="C13" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="4">
+      <c r="C14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="4">
+      <c r="C15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="4">
+      <c r="C16" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="18"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="4">
+      <c r="C17" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="18"/>
+      <c r="C18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="4">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="19"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="10"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="3"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="10">
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>